<commit_message>
Measured Packet Processing time for 4 switches
Updated the summary excel sheet as well as plot.
Added traces for 4 switches.

Signed-off-by:Ashish Kashinath<akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/SwitchProcessingTime/Summary_At1sec.xlsx
+++ b/SwitchProcessingTime/Summary_At1sec.xlsx
@@ -23,12 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
   <si>
     <t>Two Switch</t>
-  </si>
-  <si>
-    <t>One</t>
   </si>
   <si>
     <t>Worst Case</t>
@@ -53,6 +50,21 @@
   </si>
   <si>
     <t>(Standard Dev/Mean) expressed in %</t>
+  </si>
+  <si>
+    <t>Three Switches(us)</t>
+  </si>
+  <si>
+    <t>Four Switches(us)</t>
+  </si>
+  <si>
+    <t>Three Switch</t>
+  </si>
+  <si>
+    <t>Four Switch</t>
+  </si>
+  <si>
+    <t>One Switch</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -139,6 +151,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,13 +459,14 @@
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
+      <selection pane="bottomLeft" activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
@@ -439,7 +474,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2450,23 +2485,39 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
+      <c r="B103" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C103" s="3"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
+      <c r="F103" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
+      <c r="B104">
+        <v>527.51400000000001</v>
+      </c>
+      <c r="C104">
+        <v>550.10500000000002</v>
+      </c>
+      <c r="D104">
+        <v>548.49400000000003</v>
+      </c>
       <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
+      <c r="F104">
+        <v>558.16200000000003</v>
+      </c>
+      <c r="G104">
+        <v>523.41800000000001</v>
+      </c>
+      <c r="H104">
+        <v>554.02599999999995</v>
+      </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
@@ -2519,15 +2570,17 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="12"/>
-    <col min="6" max="6" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="12"/>
     <col min="7" max="7" width="31.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="12"/>
   </cols>
@@ -2535,235 +2588,296 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9"/>
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7">
+        <v>598.30200000000002</v>
+      </c>
+      <c r="C2" s="7">
         <v>573.61599999999999</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
-        <v>598.30200000000002</v>
-      </c>
+      <c r="D2" s="20">
+        <v>634.34</v>
+      </c>
+      <c r="E2" s="20">
+        <v>637.58000000000004</v>
+      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7">
+        <v>553.89400000000001</v>
+      </c>
+      <c r="C3" s="7">
         <v>578.83500000000004</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
-        <v>553.89400000000001</v>
-      </c>
+      <c r="D3" s="20">
+        <v>566.87099999999998</v>
+      </c>
+      <c r="E3" s="12">
+        <v>642.24099999999999</v>
+      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
+        <v>544.51499999999999</v>
+      </c>
+      <c r="C4" s="7">
         <v>604.18299999999999</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
-        <v>544.51499999999999</v>
-      </c>
+      <c r="D4" s="20">
+        <v>656.75099999999998</v>
+      </c>
+      <c r="E4" s="12">
+        <v>630.08500000000004</v>
+      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="7">
+        <v>580.48699999999997</v>
+      </c>
+      <c r="C5" s="7">
         <v>627.62900000000002</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
-        <v>580.48699999999997</v>
-      </c>
+      <c r="D5" s="20">
+        <v>624.53099999999995</v>
+      </c>
+      <c r="E5" s="20">
+        <v>583.26800000000003</v>
+      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="7">
+        <v>556.995</v>
+      </c>
+      <c r="C6" s="7">
         <v>580.62699999999995</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
-        <v>556.995</v>
-      </c>
+      <c r="D6" s="20">
+        <v>623.47199999999998</v>
+      </c>
+      <c r="E6" s="20">
+        <v>632.25699999999995</v>
+      </c>
+      <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="7">
+        <v>534.26300000000003</v>
+      </c>
+      <c r="C7" s="7">
         <v>585.42200000000003</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
-        <v>534.26300000000003</v>
-      </c>
+      <c r="D7" s="20">
+        <v>613.673</v>
+      </c>
+      <c r="E7" s="20">
+        <v>629.09900000000005</v>
+      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="7">
+        <v>560.923</v>
+      </c>
+      <c r="C8" s="7">
         <v>654.62199999999996</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7">
-        <v>560.923</v>
-      </c>
+      <c r="D8" s="20">
+        <v>604.91800000000001</v>
+      </c>
+      <c r="E8" s="20">
+        <v>623.31799999999998</v>
+      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="7">
+        <v>581.80999999999995</v>
+      </c>
+      <c r="C9" s="7">
         <v>581.07100000000003</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7">
-        <v>581.80999999999995</v>
-      </c>
+      <c r="D9" s="20">
+        <v>635.96</v>
+      </c>
+      <c r="E9" s="20">
+        <v>651.32399999999996</v>
+      </c>
+      <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="7">
+        <v>559.37599999999998</v>
+      </c>
+      <c r="C10" s="7">
         <v>638.54399999999998</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7">
-        <v>559.37599999999998</v>
-      </c>
+      <c r="D10" s="20">
+        <v>613.12599999999998</v>
+      </c>
+      <c r="E10" s="20">
+        <v>583.46799999999996</v>
+      </c>
+      <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="7">
+        <v>533.69100000000003</v>
+      </c>
+      <c r="C11" s="7">
         <v>588.18399999999997</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7">
-        <v>533.69100000000003</v>
-      </c>
+      <c r="D11" s="20">
+        <v>593.79</v>
+      </c>
+      <c r="E11" s="20">
+        <v>628.81700000000001</v>
+      </c>
+      <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="7">
         <f>AVERAGE(B2:B11)</f>
+        <v>560.42560000000003</v>
+      </c>
+      <c r="C13" s="7">
+        <f>AVERAGE(C2:C11)</f>
         <v>601.27330000000006</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7">
-        <f>AVERAGE(F2:F11)</f>
-        <v>560.42560000000003</v>
-      </c>
+      <c r="D13" s="12">
+        <f>AVERAGE(D2:D11)</f>
+        <v>616.7432</v>
+      </c>
+      <c r="E13" s="12">
+        <f>AVERAGE(E2:E11)</f>
+        <v>624.14569999999992</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
-        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <f t="shared" ref="B14" si="0">_xlfn.STDEV.P(B2:B11)</f>
+        <v>20.006302907833806</v>
+      </c>
+      <c r="C14" s="7">
+        <f>_xlfn.STDEV.P(C2:C11)</f>
         <v>27.319732451288747</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7">
-        <f t="shared" ref="F14" si="0">_xlfn.STDEV.P(F2:F11)</f>
-        <v>20.006302907833806</v>
-      </c>
+      <c r="D14" s="12">
+        <f>_xlfn.STDEV.P(D2:D11)</f>
+        <v>23.583712077618319</v>
+      </c>
+      <c r="E14" s="12">
+        <f>_xlfn.STDEV.P(E2:E11)</f>
+        <v>21.726370401196789</v>
+      </c>
+      <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="7">
-        <f>B14*100/B13</f>
+        <f t="shared" ref="B15" si="1">B14*100/B13</f>
+        <v>3.5698410115158561</v>
+      </c>
+      <c r="C15" s="7">
+        <f>C14*100/C13</f>
         <v>4.5436463670162546</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7">
-        <f t="shared" ref="F15" si="1">F14*100/F13</f>
-        <v>3.5698410115158561</v>
-      </c>
+      <c r="D15" s="12">
+        <f>D14*100/D13</f>
+        <v>3.8239111639363546</v>
+      </c>
+      <c r="E15" s="12">
+        <f>E14*100/E13</f>
+        <v>3.4809773425014052</v>
+      </c>
+      <c r="F15" s="7"/>
       <c r="G15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="14">
-        <f>(B13-F13)</f>
-        <v>40.847700000000032</v>
+        <v>3</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="E16" s="12">
+        <f>(E13-B13)/3</f>
+        <v>21.240033333333297</v>
       </c>
     </row>
   </sheetData>
@@ -2776,400 +2890,453 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7">
+        <v>589.79499999999996</v>
+      </c>
+      <c r="C2" s="7">
         <v>519.84400000000005</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
-        <v>589.79499999999996</v>
-      </c>
+      <c r="D2" s="15">
+        <v>506.86399999999998</v>
+      </c>
+      <c r="E2" s="18">
+        <v>518.553</v>
+      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7">
+        <v>508.32</v>
+      </c>
+      <c r="C3" s="7">
         <v>520.19600000000003</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
-        <v>508.32</v>
-      </c>
+      <c r="D3" s="16">
+        <v>540.88599999999997</v>
+      </c>
+      <c r="E3" s="18">
+        <v>482.02800000000002</v>
+      </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
+        <v>457.11399999999998</v>
+      </c>
+      <c r="C4" s="7">
         <v>510.81299999999999</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
-        <v>457.11399999999998</v>
-      </c>
+      <c r="D4" s="15">
+        <v>519.423</v>
+      </c>
+      <c r="E4" s="19">
+        <v>535.53200000000004</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="7">
+        <v>498.12700000000001</v>
+      </c>
+      <c r="C5" s="7">
         <v>503.85300000000001</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
-        <v>498.12700000000001</v>
-      </c>
+      <c r="D5" s="15">
+        <v>555.923</v>
+      </c>
+      <c r="E5" s="18">
+        <v>529.351</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="7">
+        <v>561.79899999999998</v>
+      </c>
+      <c r="C6" s="7">
         <v>506.60899999999998</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
-        <v>561.79899999999998</v>
-      </c>
+      <c r="D6" s="15">
+        <v>543.85900000000004</v>
+      </c>
+      <c r="E6" s="18">
+        <v>561.32000000000005</v>
+      </c>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="7">
+        <v>430.54500000000002</v>
+      </c>
+      <c r="C7" s="7">
         <v>501.53</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
-        <v>430.54500000000002</v>
-      </c>
+      <c r="D7" s="15">
+        <v>530.25900000000001</v>
+      </c>
+      <c r="E7" s="18">
+        <v>523.899</v>
+      </c>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="7">
+        <v>440.142</v>
+      </c>
+      <c r="C8" s="7">
         <v>486.84899999999999</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7">
-        <v>440.142</v>
-      </c>
+      <c r="D8" s="15">
+        <v>556.46699999999998</v>
+      </c>
+      <c r="E8" s="18">
+        <v>540.25</v>
+      </c>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="7">
-        <f>AVERAGE(B2:B8,'1024B_at_1sec'!B102:D102)</f>
+        <f>AVERAGE(B2:B8,Sheet1!F101:H101)</f>
+        <v>490.78407171717174</v>
+      </c>
+      <c r="C10" s="7">
+        <f>AVERAGE(C2:C8,'1024B_at_1sec'!C102:E102)</f>
         <v>507.09914285714291</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7">
-        <f>AVERAGE(F2:F8,Sheet1!F101:H101)</f>
-        <v>490.78407171717174</v>
-      </c>
+      <c r="D10" s="16">
+        <f>AVERAGE(D2:D8,'1024B_at_1sec'!B104:D104)</f>
+        <v>536.24014285714281</v>
+      </c>
+      <c r="E10" s="19">
+        <f>AVERAGE(E2:E8,Sheet1!F104:H104)</f>
+        <v>532.65390000000002</v>
+      </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="7">
-        <f>_xlfn.STDEV.P(B2:B8,Sheet1!B101:D101)</f>
+        <f>_xlfn.STDEV.P(B2:B8,Sheet1!F101:H101)</f>
+        <v>70.458516442947058</v>
+      </c>
+      <c r="C11" s="7">
+        <f>_xlfn.STDEV.P(C2:C8,Sheet1!B101:D101)</f>
         <v>40.441137614408753</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7">
-        <f>_xlfn.STDEV.P(F2:F8,Sheet1!F101:H101)</f>
-        <v>70.458516442947058</v>
-      </c>
+      <c r="D11" s="16">
+        <f>_xlfn.STDEV.P(D2:D8,'1024B_at_1sec'!B104:D104)</f>
+        <v>17.145260573186082</v>
+      </c>
+      <c r="E11" s="19">
+        <f>_xlfn.STDEV.P(E2:E8,Sheet1!F104:H104)</f>
+        <v>22.203233347645565</v>
+      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="7">
-        <f>B11*100/B10</f>
+        <f t="shared" ref="B12" si="0">B11*100/B10</f>
+        <v>14.356316861797174</v>
+      </c>
+      <c r="C12" s="7">
+        <f>C11*100/C10</f>
         <v>7.9749962475881366</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7">
-        <f t="shared" ref="F12" si="0">F11*100/F10</f>
-        <v>14.356316861797174</v>
-      </c>
+      <c r="D12" s="16">
+        <f>D11*100/D10</f>
+        <v>3.197310160674351</v>
+      </c>
+      <c r="E12" s="19">
+        <f>E11*100/E10</f>
+        <v>4.1684165548483856</v>
+      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="69.75" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5">
-        <f>(B10-F10)</f>
-        <v>16.315071139971167</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13">
+        <f>(E10-B10)/3</f>
+        <v>13.956609427609427</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="7"/>
-    <col min="6" max="6" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="9"/>
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>495.93400000000003</v>
+      </c>
+      <c r="C2" s="7">
+        <v>504.21499999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>483.62099999999998</v>
+      </c>
+      <c r="C3" s="7">
+        <v>530.30100000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>501.38900000000001</v>
+      </c>
+      <c r="C4" s="7">
+        <v>489.51600000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>499.44200000000001</v>
+      </c>
+      <c r="C5" s="7">
+        <v>505.58699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>477.87700000000001</v>
+      </c>
+      <c r="C6" s="7">
+        <v>454.37700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>508.73599999999999</v>
+      </c>
+      <c r="C7" s="7">
+        <v>493.75900000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>473.11500000000001</v>
+      </c>
+      <c r="C8" s="7">
+        <v>497.88099999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>491.59</v>
+      </c>
+      <c r="C9" s="7">
+        <v>515.774</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>493.42</v>
+      </c>
+      <c r="C10" s="7">
+        <v>523.22299999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
+        <v>424.351</v>
+      </c>
+      <c r="C11" s="7">
+        <v>506.71199999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="7">
-        <v>504.21499999999997</v>
-      </c>
-      <c r="F2" s="7">
-        <v>495.93400000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>530.30100000000004</v>
-      </c>
-      <c r="F3" s="7">
-        <v>483.62099999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7">
-        <v>489.51600000000002</v>
-      </c>
-      <c r="F4" s="7">
-        <v>501.38900000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7">
-        <v>505.58699999999999</v>
-      </c>
-      <c r="F5" s="7">
-        <v>499.44200000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="7">
-        <v>454.37700000000001</v>
-      </c>
-      <c r="F6" s="7">
-        <v>477.87700000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7">
-        <v>493.75900000000001</v>
-      </c>
-      <c r="F7" s="7">
-        <v>508.73599999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="7">
-        <v>497.88099999999997</v>
-      </c>
-      <c r="F8" s="7">
-        <v>473.11500000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7">
-        <v>515.774</v>
-      </c>
-      <c r="F9" s="7">
-        <v>491.59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="7">
-        <v>523.22299999999996</v>
-      </c>
-      <c r="F10" s="7">
-        <v>493.42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="7">
-        <v>506.71199999999999</v>
-      </c>
-      <c r="F11" s="7">
-        <v>424.351</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>3</v>
       </c>
       <c r="B13" s="7">
         <f>AVERAGE(B2:B11)</f>
+        <v>484.94749999999993</v>
+      </c>
+      <c r="C13" s="7">
+        <f>AVERAGE(C2:C11)</f>
         <v>502.13449999999995</v>
       </c>
-      <c r="F13" s="7">
-        <f>AVERAGE(F2:F11)</f>
-        <v>484.94749999999993</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
-        <f>_xlfn.STDEV.P(B5:B11,Sheet1!B104:D104)</f>
-        <v>20.6614176835443</v>
-      </c>
-      <c r="F14" s="7">
-        <f>_xlfn.STDEV.P(F5:F11,Sheet1!F104:H104)</f>
-        <v>25.791743594271654</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <v>22.686143062451144</v>
+      </c>
+      <c r="C14" s="7">
+        <f>_xlfn.STDEV.P(C2:C11)</f>
+        <v>19.973885121578125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="7">
-        <f>B14*100/B13</f>
-        <v>4.1147178063933669</v>
-      </c>
-      <c r="F15" s="7">
-        <f t="shared" ref="F15" si="0">F14*100/F13</f>
-        <v>5.3184609868638688</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B15" si="0">B14*100/B13</f>
+        <v>4.6780616587261807</v>
+      </c>
+      <c r="C15" s="7">
+        <f>C14*100/C13</f>
+        <v>3.9777958139857206</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="11">
-        <f>(B13-F13)</f>
+        <v>3</v>
+      </c>
+      <c r="C16" s="11">
+        <f>(C13-B13)</f>
         <v>17.187000000000012</v>
       </c>
     </row>
@@ -3184,189 +3351,285 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="7"/>
-    <col min="6" max="6" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7"/>
     <col min="7" max="7" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7">
+        <v>304.40199999999999</v>
+      </c>
+      <c r="C2" s="7">
         <v>305.10000000000002</v>
       </c>
-      <c r="F2" s="7">
-        <v>304.40199999999999</v>
+      <c r="D2" s="15">
+        <v>352.89100000000002</v>
+      </c>
+      <c r="E2" s="15">
+        <v>496.38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7">
+        <v>296.91000000000003</v>
+      </c>
+      <c r="C3" s="7">
         <v>292.14499999999998</v>
       </c>
-      <c r="F3" s="7">
-        <v>296.91000000000003</v>
+      <c r="D3" s="15">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="E3" s="16">
+        <v>294.173</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
+        <v>311.524</v>
+      </c>
+      <c r="C4" s="7">
         <v>316.82799999999997</v>
       </c>
-      <c r="F4" s="7">
-        <v>311.524</v>
+      <c r="D4" s="15">
+        <v>356.839</v>
+      </c>
+      <c r="E4" s="15">
+        <v>335.15699999999998</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="7">
+        <v>282.04500000000002</v>
+      </c>
+      <c r="C5" s="7">
         <v>299.51299999999998</v>
       </c>
-      <c r="F5" s="7">
-        <v>282.04500000000002</v>
+      <c r="D5" s="15">
+        <v>320.06099999999998</v>
+      </c>
+      <c r="E5" s="15">
+        <v>338.95299999999997</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="7">
+        <v>315.12400000000002</v>
+      </c>
+      <c r="C6" s="7">
         <v>316.92</v>
       </c>
-      <c r="F6" s="7">
-        <v>315.12400000000002</v>
+      <c r="D6" s="16">
+        <v>362.31400000000002</v>
+      </c>
+      <c r="E6" s="15">
+        <v>356.96600000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="7">
+        <v>283.71199999999999</v>
+      </c>
+      <c r="C7" s="7">
         <v>306.84800000000001</v>
       </c>
-      <c r="F7" s="7">
-        <v>283.71199999999999</v>
+      <c r="D7" s="15">
+        <v>325.887</v>
+      </c>
+      <c r="E7" s="15">
+        <v>277.16000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="7">
+        <v>314.13499999999999</v>
+      </c>
+      <c r="C8" s="7">
         <v>324.21800000000002</v>
       </c>
-      <c r="F8" s="7">
-        <v>314.13499999999999</v>
+      <c r="D8" s="15">
+        <v>332.31400000000002</v>
+      </c>
+      <c r="E8" s="15">
+        <v>342.43700000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="7">
+        <v>318.67099999999999</v>
+      </c>
+      <c r="C9" s="7">
         <v>326.17399999999998</v>
       </c>
-      <c r="F9" s="7">
-        <v>318.67099999999999</v>
+      <c r="D9" s="15">
+        <v>324.04399999999998</v>
+      </c>
+      <c r="E9" s="15">
+        <v>353.15300000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="7">
+        <v>290.21199999999999</v>
+      </c>
+      <c r="C10" s="7">
         <v>322.88200000000001</v>
       </c>
-      <c r="F10" s="7">
-        <v>290.21199999999999</v>
+      <c r="D10" s="16">
+        <v>338.89400000000001</v>
+      </c>
+      <c r="E10" s="15">
+        <v>345.166</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="7">
+        <v>310.02999999999997</v>
+      </c>
+      <c r="C11" s="7">
         <v>308.44900000000001</v>
       </c>
-      <c r="F11" s="7">
-        <v>310.02999999999997</v>
-      </c>
+      <c r="D11" s="16">
+        <v>355.67</v>
+      </c>
+      <c r="E11" s="15">
+        <v>328.02499999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="7">
         <f>AVERAGE(B2:B11)</f>
+        <v>302.67649999999992</v>
+      </c>
+      <c r="C13" s="7">
+        <f>AVERAGE(C2:C11)</f>
         <v>311.90770000000003</v>
       </c>
-      <c r="F13" s="7">
-        <f>AVERAGE(F2:F11)</f>
-        <v>302.67649999999992</v>
+      <c r="D13" s="16">
+        <f>AVERAGE(D2:D11)</f>
+        <v>336.23139999999995</v>
+      </c>
+      <c r="E13" s="16">
+        <f>AVERAGE(E2:E11)</f>
+        <v>346.75700000000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
-        <f>_xlfn.STDEV.P(B5:B11,Sheet1!B104:D104)</f>
-        <v>9.4480534330342056</v>
-      </c>
-      <c r="F14" s="7">
-        <f>_xlfn.STDEV.P(F5:F11,Sheet1!F104:H104)</f>
-        <v>14.801109682612809</v>
+        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <v>12.850363467622227</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" ref="C14:E14" si="0">_xlfn.STDEV.P(C2:C11)</f>
+        <v>10.737501637252498</v>
+      </c>
+      <c r="D14" s="16">
+        <f t="shared" si="0"/>
+        <v>20.33313083713378</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>55.415284905881322</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="7">
-        <f>B14*100/B13</f>
-        <v>3.0291183683616034</v>
-      </c>
-      <c r="F15" s="7">
-        <f t="shared" ref="F15" si="0">F14*100/F13</f>
-        <v>4.8900756030325487</v>
+        <f t="shared" ref="B15" si="1">B14*100/B13</f>
+        <v>4.2455768675870873</v>
+      </c>
+      <c r="C15" s="7">
+        <f>C14*100/C13</f>
+        <v>3.442525348765836</v>
+      </c>
+      <c r="D15" s="16">
+        <f>D14*100/D13</f>
+        <v>6.0473622740570283</v>
+      </c>
+      <c r="E15" s="16">
+        <f>E14*100/E13</f>
+        <v>15.981014054764959</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="11">
-        <f>(B13-F13)</f>
-        <v>9.2312000000001149</v>
+        <v>3</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11">
+        <f>(E13-B13)/3</f>
+        <v>14.693500000000029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Average case numbers to RPi excel sheet
Also changing the name of the laptop measurement
excel sheet to laptop_measurements_100ms

Signed-off-by:Ashish Kashinath<akashina@eng.ucsd.edu>
</commit_message>
<xml_diff>
--- a/SwitchProcessingTime/Summary_At1sec.xlsx
+++ b/SwitchProcessingTime/Summary_At1sec.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="499" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="1408B_at_1sec" sheetId="5" r:id="rId2"/>
-    <sheet name="1024B_at_1sec" sheetId="2" r:id="rId3"/>
-    <sheet name="512B_at_1sec" sheetId="3" r:id="rId4"/>
-    <sheet name="256B_at_1sec" sheetId="4" r:id="rId5"/>
+    <sheet name="256B_at_1sec" sheetId="4" r:id="rId2"/>
+    <sheet name="512B_at_1sec" sheetId="3" r:id="rId3"/>
+    <sheet name="1024B_at_1sec" sheetId="2" r:id="rId4"/>
+    <sheet name="1408B_at_1sec" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="15">
   <si>
     <t>Two Switch</t>
   </si>
@@ -49,9 +49,6 @@
     <t>One-switch(us)</t>
   </si>
   <si>
-    <t>(Standard Dev/Mean) expressed in %</t>
-  </si>
-  <si>
     <t>Three Switches(us)</t>
   </si>
   <si>
@@ -65,6 +62,12 @@
   </si>
   <si>
     <t>One Switch</t>
+  </si>
+  <si>
+    <t>Average Case</t>
+  </si>
+  <si>
+    <t>Average of Average Cases</t>
   </si>
 </sst>
 </file>
@@ -95,12 +98,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -174,6 +183,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,7 +499,7 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
@@ -2486,13 +2511,13 @@
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
@@ -2567,10 +2592,1401 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="7"/>
+    <col min="7" max="7" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="G1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>304.40199999999999</v>
+      </c>
+      <c r="D3" s="15">
+        <v>352.89100000000002</v>
+      </c>
+      <c r="E3" s="15">
+        <v>496.38</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="7">
+        <v>249.71899999999999</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3">
+        <v>273.13400000000001</v>
+      </c>
+      <c r="K3">
+        <v>266.59399999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>296.91000000000003</v>
+      </c>
+      <c r="C4" s="7">
+        <v>292.14499999999998</v>
+      </c>
+      <c r="D4" s="15">
+        <v>293.39999999999998</v>
+      </c>
+      <c r="E4" s="16">
+        <v>294.173</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="7">
+        <v>243.88300000000001</v>
+      </c>
+      <c r="I4">
+        <v>236.68299999999999</v>
+      </c>
+      <c r="J4">
+        <v>262.83</v>
+      </c>
+      <c r="K4">
+        <v>260.46199999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>311.524</v>
+      </c>
+      <c r="C5" s="7">
+        <v>316.82799999999997</v>
+      </c>
+      <c r="D5" s="15">
+        <v>356.839</v>
+      </c>
+      <c r="E5" s="15">
+        <v>335.15699999999998</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="7">
+        <v>254.39</v>
+      </c>
+      <c r="I5">
+        <v>243.131</v>
+      </c>
+      <c r="J5">
+        <v>270.84199999999998</v>
+      </c>
+      <c r="K5">
+        <v>266.87400000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>282.04500000000002</v>
+      </c>
+      <c r="C6" s="7">
+        <v>299.51299999999998</v>
+      </c>
+      <c r="D6" s="15">
+        <v>320.06099999999998</v>
+      </c>
+      <c r="E6" s="15">
+        <v>338.95299999999997</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="7">
+        <v>238.16800000000001</v>
+      </c>
+      <c r="I6">
+        <v>232.26400000000001</v>
+      </c>
+      <c r="J6">
+        <v>267.00700000000001</v>
+      </c>
+      <c r="K6">
+        <v>277.14699999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>315.12400000000002</v>
+      </c>
+      <c r="C7" s="7">
+        <v>316.92</v>
+      </c>
+      <c r="D7" s="16">
+        <v>362.31400000000002</v>
+      </c>
+      <c r="E7" s="15">
+        <v>356.96600000000001</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="7">
+        <v>243.53299999999999</v>
+      </c>
+      <c r="I7">
+        <v>238.91499999999999</v>
+      </c>
+      <c r="J7">
+        <v>282.56599999999997</v>
+      </c>
+      <c r="K7">
+        <v>274.89100000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>283.71199999999999</v>
+      </c>
+      <c r="C8" s="7">
+        <v>306.84800000000001</v>
+      </c>
+      <c r="D8" s="15">
+        <v>325.887</v>
+      </c>
+      <c r="E8" s="15">
+        <v>277.16000000000003</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="7">
+        <v>235.12</v>
+      </c>
+      <c r="I8">
+        <v>247.43700000000001</v>
+      </c>
+      <c r="J8">
+        <v>262.98899999999998</v>
+      </c>
+      <c r="K8">
+        <v>242.55600000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>314.13499999999999</v>
+      </c>
+      <c r="C9" s="7">
+        <v>324.21800000000002</v>
+      </c>
+      <c r="D9" s="15">
+        <v>332.31400000000002</v>
+      </c>
+      <c r="E9" s="15">
+        <v>342.43700000000001</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="7">
+        <v>248.18100000000001</v>
+      </c>
+      <c r="I9">
+        <v>255.65799999999999</v>
+      </c>
+      <c r="J9">
+        <v>272.62599999999998</v>
+      </c>
+      <c r="K9">
+        <v>271.80399999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>318.67099999999999</v>
+      </c>
+      <c r="C10" s="7">
+        <v>326.17399999999998</v>
+      </c>
+      <c r="D10" s="15">
+        <v>324.04399999999998</v>
+      </c>
+      <c r="E10" s="15">
+        <v>353.15300000000002</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="7">
+        <v>241.28</v>
+      </c>
+      <c r="I10">
+        <v>235.36799999999999</v>
+      </c>
+      <c r="J10">
+        <v>264.02100000000002</v>
+      </c>
+      <c r="K10">
+        <v>280.43700000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
+        <v>290.21199999999999</v>
+      </c>
+      <c r="C11" s="7">
+        <v>322.88200000000001</v>
+      </c>
+      <c r="D11" s="16">
+        <v>338.89400000000001</v>
+      </c>
+      <c r="E11" s="15">
+        <v>345.166</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="7">
+        <v>228.88200000000001</v>
+      </c>
+      <c r="I11">
+        <v>261.464</v>
+      </c>
+      <c r="J11">
+        <v>257.36099999999999</v>
+      </c>
+      <c r="K11">
+        <v>280.90300000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
+        <v>310.02999999999997</v>
+      </c>
+      <c r="C12" s="7">
+        <v>308.44900000000001</v>
+      </c>
+      <c r="D12" s="16">
+        <v>355.67</v>
+      </c>
+      <c r="E12" s="15">
+        <v>328.02499999999998</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="7">
+        <v>243.27699999999999</v>
+      </c>
+      <c r="I12">
+        <v>241.40700000000001</v>
+      </c>
+      <c r="J12">
+        <v>273.87900000000002</v>
+      </c>
+      <c r="K12">
+        <v>261.02499999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="24"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7">
+        <f>AVERAGE(B3:B12)</f>
+        <v>302.67649999999992</v>
+      </c>
+      <c r="C14" s="7">
+        <f>AVERAGE(C3:C12)</f>
+        <v>312.66411111111108</v>
+      </c>
+      <c r="D14" s="16">
+        <f>AVERAGE(D3:D12)</f>
+        <v>336.23139999999995</v>
+      </c>
+      <c r="E14" s="16">
+        <f>AVERAGE(E3:E12)</f>
+        <v>346.75700000000001</v>
+      </c>
+      <c r="F14" s="24"/>
+      <c r="G14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="7">
+        <f>AVERAGE(H3:H12)</f>
+        <v>242.64330000000001</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" ref="I14:K14" si="0">AVERAGE(I3:I12)</f>
+        <v>243.59188888888886</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="0"/>
+        <v>268.72549999999995</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="0"/>
+        <v>268.26929999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7">
+        <f>_xlfn.STDEV.P(B3:B12)</f>
+        <v>12.850363467622227</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" ref="C15:E15" si="1">_xlfn.STDEV.P(C3:C12)</f>
+        <v>11.062676062071107</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" si="1"/>
+        <v>20.33313083713378</v>
+      </c>
+      <c r="E15" s="16">
+        <f t="shared" si="1"/>
+        <v>55.415284905881322</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="7">
+        <f>_xlfn.STDEV.P(H3:H12)</f>
+        <v>6.9950477346477022</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" ref="I15:K15" si="2">_xlfn.STDEV.P(I3:I12)</f>
+        <v>9.130741000043562</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="2"/>
+        <v>6.9220526038162982</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="2"/>
+        <v>11.055220378174289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7">
+        <f t="shared" ref="B16" si="3">B15*100/B14</f>
+        <v>4.2455768675870873</v>
+      </c>
+      <c r="C16" s="7">
+        <f>C15*100/C14</f>
+        <v>3.5381982354027759</v>
+      </c>
+      <c r="D16" s="16">
+        <f>D15*100/D14</f>
+        <v>6.0473622740570283</v>
+      </c>
+      <c r="E16" s="16">
+        <f>E15*100/E14</f>
+        <v>15.981014054764959</v>
+      </c>
+      <c r="F16" s="24"/>
+      <c r="G16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="7">
+        <f>(H15*100)/H14</f>
+        <v>2.8828522092502458</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" ref="I16:K16" si="4">(I15*100)/I14</f>
+        <v>3.7483764511586122</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="4"/>
+        <v>2.5758823051092286</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="4"/>
+        <v>4.120941299721693</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11">
+        <f>(E14-B14)/3</f>
+        <v>14.693500000000029</v>
+      </c>
+      <c r="F17" s="24"/>
+      <c r="G17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11">
+        <f>(K14-H14)/3</f>
+        <v>8.5419999999999927</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="7"/>
+    <col min="5" max="5" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="E1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="F2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>495.93400000000003</v>
+      </c>
+      <c r="C3" s="7">
+        <v>504.21499999999997</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>421.59800000000001</v>
+      </c>
+      <c r="G3">
+        <v>438.85700000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>483.62099999999998</v>
+      </c>
+      <c r="C4" s="7">
+        <v>530.30100000000004</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>414.62799999999999</v>
+      </c>
+      <c r="G4">
+        <v>411.03399999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>501.38900000000001</v>
+      </c>
+      <c r="C5" s="7">
+        <v>489.51600000000002</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>410.79399999999998</v>
+      </c>
+      <c r="G5">
+        <v>432.36599999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>499.44200000000001</v>
+      </c>
+      <c r="C6" s="7">
+        <v>505.58699999999999</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>416.29500000000002</v>
+      </c>
+      <c r="G6">
+        <v>415.065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>477.87700000000001</v>
+      </c>
+      <c r="C7" s="7">
+        <v>454.37700000000001</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>404.20400000000001</v>
+      </c>
+      <c r="G7">
+        <v>406.38299999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>508.73599999999999</v>
+      </c>
+      <c r="C8" s="7">
+        <v>493.75900000000001</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>427.09500000000003</v>
+      </c>
+      <c r="G8">
+        <v>429.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>473.11500000000001</v>
+      </c>
+      <c r="C9" s="7">
+        <v>497.88099999999997</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>394.35700000000003</v>
+      </c>
+      <c r="G9">
+        <v>437.70499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>491.59</v>
+      </c>
+      <c r="C10" s="7">
+        <v>515.774</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>394.82</v>
+      </c>
+      <c r="G10">
+        <v>425.43099999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7">
+        <v>493.42</v>
+      </c>
+      <c r="C11" s="7">
+        <v>523.22299999999996</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>417.28699999999998</v>
+      </c>
+      <c r="G11">
+        <v>432.99200000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
+        <v>424.351</v>
+      </c>
+      <c r="C12" s="7">
+        <v>506.71199999999999</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>392.71499999999997</v>
+      </c>
+      <c r="G12">
+        <v>433.75400000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="24"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="7">
+        <f>AVERAGE(B3:B12)</f>
+        <v>484.94749999999993</v>
+      </c>
+      <c r="C14" s="7">
+        <f>AVERAGE(C3:C12)</f>
+        <v>502.13449999999995</v>
+      </c>
+      <c r="D14" s="24"/>
+      <c r="E14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="7">
+        <f>AVERAGE(F3:F12)</f>
+        <v>409.37930000000006</v>
+      </c>
+      <c r="G14" s="7">
+        <f>AVERAGE(G3:G12)</f>
+        <v>426.26670000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7">
+        <f>_xlfn.STDEV.P(B3:B12)</f>
+        <v>22.686143062451144</v>
+      </c>
+      <c r="C15" s="7">
+        <f>_xlfn.STDEV.P(C3:C12)</f>
+        <v>19.973885121578125</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7">
+        <f>_xlfn.STDEV.P(F3:F12)</f>
+        <v>11.598175925980781</v>
+      </c>
+      <c r="G15" s="7">
+        <f>_xlfn.STDEV.P(G3:G12)</f>
+        <v>10.905635937899273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7">
+        <f t="shared" ref="B16" si="0">B15*100/B14</f>
+        <v>4.6780616587261807</v>
+      </c>
+      <c r="C16" s="7">
+        <f>C15*100/C14</f>
+        <v>3.9777958139857206</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="7">
+        <f>(F15*100)/F14</f>
+        <v>2.833112452432446</v>
+      </c>
+      <c r="G16" s="7">
+        <f>(G15*100)/G14</f>
+        <v>2.5584067293784085</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="11">
+        <f>(C14-B14)</f>
+        <v>17.187000000000012</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11">
+        <f>(G14-F14)</f>
+        <v>16.887399999999957</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="G1" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>589.79499999999996</v>
+      </c>
+      <c r="C3" s="7">
+        <v>519.84400000000005</v>
+      </c>
+      <c r="D3" s="15">
+        <v>506.86399999999998</v>
+      </c>
+      <c r="E3" s="18">
+        <v>518.553</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="7">
+        <v>416.71499999999997</v>
+      </c>
+      <c r="I3">
+        <v>429.339</v>
+      </c>
+      <c r="J3">
+        <v>457.55</v>
+      </c>
+      <c r="K3">
+        <v>455.464</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>508.32</v>
+      </c>
+      <c r="C4" s="7">
+        <v>520.19600000000003</v>
+      </c>
+      <c r="D4" s="16">
+        <v>540.88599999999997</v>
+      </c>
+      <c r="E4" s="18">
+        <v>482.02800000000002</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>422.65600000000001</v>
+      </c>
+      <c r="I4">
+        <v>415.09</v>
+      </c>
+      <c r="J4">
+        <v>472.11599999999999</v>
+      </c>
+      <c r="K4">
+        <v>441.86799999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>457.11399999999998</v>
+      </c>
+      <c r="C5" s="7">
+        <v>510.81299999999999</v>
+      </c>
+      <c r="D5" s="15">
+        <v>519.423</v>
+      </c>
+      <c r="E5" s="19">
+        <v>535.53200000000004</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>398.53699999999998</v>
+      </c>
+      <c r="I5">
+        <v>428.11200000000002</v>
+      </c>
+      <c r="J5">
+        <v>453.04899999999998</v>
+      </c>
+      <c r="K5">
+        <v>468.10899999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>498.12700000000001</v>
+      </c>
+      <c r="C6" s="7">
+        <v>503.85300000000001</v>
+      </c>
+      <c r="D6" s="15">
+        <v>555.923</v>
+      </c>
+      <c r="E6" s="18">
+        <v>529.351</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>410.24400000000003</v>
+      </c>
+      <c r="I6">
+        <v>410.68900000000002</v>
+      </c>
+      <c r="J6">
+        <v>456.41500000000002</v>
+      </c>
+      <c r="K6">
+        <v>468.28199999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>561.79899999999998</v>
+      </c>
+      <c r="C7" s="7">
+        <v>506.60899999999998</v>
+      </c>
+      <c r="D7" s="15">
+        <v>543.85900000000004</v>
+      </c>
+      <c r="E7" s="18">
+        <v>561.32000000000005</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>420.2</v>
+      </c>
+      <c r="I7">
+        <v>428.96499999999997</v>
+      </c>
+      <c r="J7">
+        <v>470.35899999999998</v>
+      </c>
+      <c r="K7">
+        <v>462.67399999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7">
+        <v>430.54500000000002</v>
+      </c>
+      <c r="C8" s="7">
+        <v>501.53</v>
+      </c>
+      <c r="D8" s="15">
+        <v>530.25900000000001</v>
+      </c>
+      <c r="E8" s="18">
+        <v>523.899</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>396.41399999999999</v>
+      </c>
+      <c r="I8" s="7">
+        <v>414.13</v>
+      </c>
+      <c r="J8">
+        <v>460.57</v>
+      </c>
+      <c r="K8">
+        <v>466.11500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>440.142</v>
+      </c>
+      <c r="C9" s="7">
+        <v>486.84899999999999</v>
+      </c>
+      <c r="D9" s="15">
+        <v>556.46699999999998</v>
+      </c>
+      <c r="E9" s="18">
+        <v>540.25</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>396.19299999999998</v>
+      </c>
+      <c r="I9">
+        <v>412.16500000000002</v>
+      </c>
+      <c r="J9">
+        <v>458.14</v>
+      </c>
+      <c r="K9">
+        <v>466.392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7">
+        <f>AVERAGE(B3:B9,Sheet1!F101:H101)</f>
+        <v>490.78407171717174</v>
+      </c>
+      <c r="C11" s="7">
+        <f>AVERAGE(C3:C9,'1024B_at_1sec'!C103:E103)</f>
+        <v>507.09914285714291</v>
+      </c>
+      <c r="D11" s="16">
+        <f>AVERAGE(D3:D9,'1024B_at_1sec'!B105:D105)</f>
+        <v>536.24014285714281</v>
+      </c>
+      <c r="E11" s="19">
+        <f>AVERAGE(E3:E9,Sheet1!F104:H104)</f>
+        <v>532.65390000000002</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="7">
+        <f>AVERAGE(H3:H9,Sheet1!L101:N101)</f>
+        <v>408.70842857142856</v>
+      </c>
+      <c r="I11" s="7">
+        <f>AVERAGE(I3:I9,'1024B_at_1sec'!I103:K103)</f>
+        <v>419.78428571428577</v>
+      </c>
+      <c r="J11" s="16">
+        <f>AVERAGE(J3:J9,'1024B_at_1sec'!H105:J105)</f>
+        <v>461.17128571428572</v>
+      </c>
+      <c r="K11" s="19">
+        <f>AVERAGE(K3:K9,Sheet1!L104:N104)</f>
+        <v>461.27199999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <f>_xlfn.STDEV.P(B3:B9,Sheet1!F101:H101)</f>
+        <v>70.458516442947058</v>
+      </c>
+      <c r="C12" s="7">
+        <f>_xlfn.STDEV.P(C3:C9,Sheet1!B101:D101)</f>
+        <v>40.441137614408753</v>
+      </c>
+      <c r="D12" s="16">
+        <f>_xlfn.STDEV.P(D3:D9,'1024B_at_1sec'!B105:D105)</f>
+        <v>17.145260573186082</v>
+      </c>
+      <c r="E12" s="19">
+        <f>_xlfn.STDEV.P(E3:E9,Sheet1!F104:H104)</f>
+        <v>22.203233347645565</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="7">
+        <f>_xlfn.STDEV.P(H3:H9,Sheet1!L101:N101)</f>
+        <v>10.719148511720817</v>
+      </c>
+      <c r="I12" s="7">
+        <f>_xlfn.STDEV.P(I3:I9,Sheet1!H101:J101)</f>
+        <v>9.4578747942217127</v>
+      </c>
+      <c r="J12" s="16">
+        <f>_xlfn.STDEV.P(J3:J9,'1024B_at_1sec'!H105:J105)</f>
+        <v>6.7130852118250681</v>
+      </c>
+      <c r="K12" s="19">
+        <f>_xlfn.STDEV.P(K3:K9,Sheet1!L104:N104)</f>
+        <v>8.9264246722061902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" ref="B13" si="0">B12*100/B11</f>
+        <v>14.356316861797174</v>
+      </c>
+      <c r="C13" s="7">
+        <f>C12*100/C11</f>
+        <v>7.9749962475881366</v>
+      </c>
+      <c r="D13" s="16">
+        <f>D12*100/D11</f>
+        <v>3.197310160674351</v>
+      </c>
+      <c r="E13" s="19">
+        <f>E12*100/E11</f>
+        <v>4.1684165548483856</v>
+      </c>
+      <c r="F13" s="24"/>
+      <c r="G13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" ref="H13" si="1">H12*100/H11</f>
+        <v>2.6226883916213315</v>
+      </c>
+      <c r="I13" s="7">
+        <f>I12*100/I11</f>
+        <v>2.2530321205636903</v>
+      </c>
+      <c r="J13" s="16">
+        <f>J12*100/J11</f>
+        <v>1.455659842617369</v>
+      </c>
+      <c r="K13" s="19">
+        <f>K12*100/K11</f>
+        <v>1.9351759205428014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14">
+        <f>(E11-B11)/3</f>
+        <v>13.956609427609427</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14">
+        <f>(K11-H11)/3</f>
+        <v>17.521190476190458</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,1057 +3998,551 @@
     <col min="5" max="5" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="12"/>
     <col min="7" max="7" width="31.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="12"/>
+    <col min="8" max="8" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="G1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>598.30200000000002</v>
-      </c>
-      <c r="C2" s="7">
-        <v>573.61599999999999</v>
-      </c>
-      <c r="D2" s="20">
-        <v>634.34</v>
-      </c>
-      <c r="E2" s="20">
-        <v>637.58000000000004</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7">
-        <v>553.89400000000001</v>
+        <v>598.30200000000002</v>
       </c>
       <c r="C3" s="7">
-        <v>578.83500000000004</v>
+        <v>573.61599999999999</v>
       </c>
       <c r="D3" s="20">
-        <v>566.87099999999998</v>
-      </c>
-      <c r="E3" s="12">
-        <v>642.24099999999999</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>634.34</v>
+      </c>
+      <c r="E3" s="20">
+        <v>637.58000000000004</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>503.26400000000001</v>
+      </c>
+      <c r="I3">
+        <v>521.29100000000005</v>
+      </c>
+      <c r="J3">
+        <v>557.42899999999997</v>
+      </c>
+      <c r="K3">
+        <v>573.72900000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="7">
-        <v>544.51499999999999</v>
+        <v>553.89400000000001</v>
       </c>
       <c r="C4" s="7">
-        <v>604.18299999999999</v>
+        <v>578.83500000000004</v>
       </c>
       <c r="D4" s="20">
-        <v>656.75099999999998</v>
+        <v>566.87099999999998</v>
       </c>
       <c r="E4" s="12">
-        <v>630.08500000000004</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>642.24099999999999</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>495.4</v>
+      </c>
+      <c r="I4">
+        <v>518.154</v>
+      </c>
+      <c r="J4">
+        <v>535.96100000000001</v>
+      </c>
+      <c r="K4">
+        <v>580.33900000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="7">
-        <v>580.48699999999997</v>
+        <v>544.51499999999999</v>
       </c>
       <c r="C5" s="7">
-        <v>627.62900000000002</v>
+        <v>604.18299999999999</v>
       </c>
       <c r="D5" s="20">
-        <v>624.53099999999995</v>
-      </c>
-      <c r="E5" s="20">
-        <v>583.26800000000003</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>656.75099999999998</v>
+      </c>
+      <c r="E5" s="12">
+        <v>630.08500000000004</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>491.29700000000003</v>
+      </c>
+      <c r="I5">
+        <v>519.84900000000005</v>
+      </c>
+      <c r="J5">
+        <v>555.12</v>
+      </c>
+      <c r="K5">
+        <v>566.62699999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="7">
-        <v>556.995</v>
+        <v>580.48699999999997</v>
       </c>
       <c r="C6" s="7">
-        <v>580.62699999999995</v>
+        <v>627.62900000000002</v>
       </c>
       <c r="D6" s="20">
-        <v>623.47199999999998</v>
+        <v>624.53099999999995</v>
       </c>
       <c r="E6" s="20">
-        <v>632.25699999999995</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>583.26800000000003</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>503.32900000000001</v>
+      </c>
+      <c r="I6">
+        <v>510.51400000000001</v>
+      </c>
+      <c r="J6">
+        <v>562.00099999999998</v>
+      </c>
+      <c r="K6">
+        <v>558.48800000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="7">
-        <v>534.26300000000003</v>
+        <v>556.995</v>
       </c>
       <c r="C7" s="7">
-        <v>585.42200000000003</v>
+        <v>580.62699999999995</v>
       </c>
       <c r="D7" s="20">
-        <v>613.673</v>
+        <v>623.47199999999998</v>
       </c>
       <c r="E7" s="20">
-        <v>629.09900000000005</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>632.25699999999995</v>
+      </c>
+      <c r="F7" s="24"/>
+      <c r="G7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>501.678</v>
+      </c>
+      <c r="I7">
+        <v>517.375</v>
+      </c>
+      <c r="J7">
+        <v>532.94200000000001</v>
+      </c>
+      <c r="K7">
+        <v>564.51300000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="7">
-        <v>560.923</v>
+        <v>534.26300000000003</v>
       </c>
       <c r="C8" s="7">
-        <v>654.62199999999996</v>
+        <v>585.42200000000003</v>
       </c>
       <c r="D8" s="20">
-        <v>604.91800000000001</v>
+        <v>613.673</v>
       </c>
       <c r="E8" s="20">
-        <v>623.31799999999998</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>629.09900000000005</v>
+      </c>
+      <c r="F8" s="24"/>
+      <c r="G8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>508.1</v>
+      </c>
+      <c r="I8">
+        <v>520.13099999999997</v>
+      </c>
+      <c r="J8">
+        <v>553.95699999999999</v>
+      </c>
+      <c r="K8">
+        <v>567.10699999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="7">
-        <v>581.80999999999995</v>
+        <v>560.923</v>
       </c>
       <c r="C9" s="7">
-        <v>581.07100000000003</v>
+        <v>654.62199999999996</v>
       </c>
       <c r="D9" s="20">
-        <v>635.96</v>
+        <v>604.91800000000001</v>
       </c>
       <c r="E9" s="20">
-        <v>651.32399999999996</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>623.31799999999998</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="G9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>495.81900000000002</v>
+      </c>
+      <c r="I9">
+        <v>518.26</v>
+      </c>
+      <c r="J9">
+        <v>543.16399999999999</v>
+      </c>
+      <c r="K9">
+        <v>563.58799999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="7">
-        <v>559.37599999999998</v>
+        <v>581.80999999999995</v>
       </c>
       <c r="C10" s="7">
-        <v>638.54399999999998</v>
+        <v>581.07100000000003</v>
       </c>
       <c r="D10" s="20">
-        <v>613.12599999999998</v>
+        <v>635.96</v>
       </c>
       <c r="E10" s="20">
-        <v>583.46799999999996</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>651.32399999999996</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10">
+        <v>500.30799999999999</v>
+      </c>
+      <c r="I10">
+        <v>515.4</v>
+      </c>
+      <c r="J10">
+        <v>537.57600000000002</v>
+      </c>
+      <c r="K10">
+        <v>574.95600000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="7">
+        <v>559.37599999999998</v>
+      </c>
+      <c r="C11" s="7">
+        <v>638.54399999999998</v>
+      </c>
+      <c r="D11" s="20">
+        <v>613.12599999999998</v>
+      </c>
+      <c r="E11" s="20">
+        <v>583.46799999999996</v>
+      </c>
+      <c r="F11" s="24"/>
+      <c r="G11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11">
+        <v>500.22199999999998</v>
+      </c>
+      <c r="I11">
+        <v>516.10400000000004</v>
+      </c>
+      <c r="J11">
+        <v>554.38</v>
+      </c>
+      <c r="K11">
+        <v>551.42200000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
         <v>533.69100000000003</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="7">
         <v>588.18399999999997</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D12" s="20">
         <v>593.79</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E12" s="20">
         <v>628.81700000000001</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="F12" s="24"/>
+      <c r="G12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>484.36</v>
+      </c>
+      <c r="I12">
+        <v>524.28</v>
+      </c>
+      <c r="J12">
+        <v>543.06100000000004</v>
+      </c>
+      <c r="K12" s="20">
+        <v>559.13199999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="7">
-        <f>AVERAGE(B2:B11)</f>
+      <c r="B14" s="7">
+        <f>AVERAGE(B3:B12)</f>
         <v>560.42560000000003</v>
       </c>
-      <c r="C13" s="7">
-        <f>AVERAGE(C2:C11)</f>
+      <c r="C14" s="7">
+        <f>AVERAGE(C3:C12)</f>
         <v>601.27330000000006</v>
       </c>
-      <c r="D13" s="12">
-        <f>AVERAGE(D2:D11)</f>
+      <c r="D14" s="12">
+        <f>AVERAGE(D3:D12)</f>
         <v>616.7432</v>
       </c>
-      <c r="E13" s="12">
-        <f>AVERAGE(E2:E11)</f>
+      <c r="E14" s="12">
+        <f>AVERAGE(E3:E12)</f>
         <v>624.14569999999992</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="7">
+        <f>AVERAGE(H3:H12)</f>
+        <v>498.37769999999989</v>
+      </c>
+      <c r="I14" s="7">
+        <f>AVERAGE(I3:I12)</f>
+        <v>518.13580000000002</v>
+      </c>
+      <c r="J14" s="12">
+        <f>AVERAGE(J3:J12)</f>
+        <v>547.55909999999994</v>
+      </c>
+      <c r="K14" s="12">
+        <f>AVERAGE(K3:K12)</f>
+        <v>565.99009999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7">
-        <f t="shared" ref="B14" si="0">_xlfn.STDEV.P(B2:B11)</f>
+      <c r="B15" s="7">
+        <f t="shared" ref="B15" si="0">_xlfn.STDEV.P(B3:B12)</f>
         <v>20.006302907833806</v>
       </c>
-      <c r="C14" s="7">
-        <f>_xlfn.STDEV.P(C2:C11)</f>
+      <c r="C15" s="7">
+        <f>_xlfn.STDEV.P(C3:C12)</f>
         <v>27.319732451288747</v>
       </c>
-      <c r="D14" s="12">
-        <f>_xlfn.STDEV.P(D2:D11)</f>
+      <c r="D15" s="12">
+        <f>_xlfn.STDEV.P(D3:D12)</f>
         <v>23.583712077618319</v>
       </c>
-      <c r="E14" s="12">
-        <f>_xlfn.STDEV.P(E2:E11)</f>
+      <c r="E15" s="12">
+        <f>_xlfn.STDEV.P(E3:E12)</f>
         <v>21.726370401196789</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="F15" s="24"/>
+      <c r="G15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" ref="H15" si="1">_xlfn.STDEV.P(H3:H12)</f>
+        <v>6.5036894613749805</v>
+      </c>
+      <c r="I15" s="7">
+        <f>_xlfn.STDEV.P(I3:I12)</f>
+        <v>3.5344247000042293</v>
+      </c>
+      <c r="J15" s="12">
+        <f>_xlfn.STDEV.P(J3:J12)</f>
+        <v>9.6850195709662739</v>
+      </c>
+      <c r="K15" s="12">
+        <f>_xlfn.STDEV.P(K3:K12)</f>
+        <v>8.1934025953812473</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="7">
-        <f t="shared" ref="B15" si="1">B14*100/B13</f>
+      <c r="B16" s="7">
+        <f t="shared" ref="B16" si="2">B15*100/B14</f>
         <v>3.5698410115158561</v>
       </c>
-      <c r="C15" s="7">
-        <f>C14*100/C13</f>
+      <c r="C16" s="7">
+        <f>C15*100/C14</f>
         <v>4.5436463670162546</v>
       </c>
-      <c r="D15" s="12">
-        <f>D14*100/D13</f>
+      <c r="D16" s="12">
+        <f>D15*100/D14</f>
         <v>3.8239111639363546</v>
       </c>
-      <c r="E15" s="12">
-        <f>E14*100/E13</f>
+      <c r="E16" s="12">
+        <f>E15*100/E14</f>
         <v>3.4809773425014052</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" ref="H16" si="3">H15*100/H14</f>
+        <v>1.3049720044406043</v>
+      </c>
+      <c r="I16" s="7">
+        <f>I15*100/I14</f>
+        <v>0.68214253869434016</v>
+      </c>
+      <c r="J16" s="12">
+        <f>J15*100/J14</f>
+        <v>1.7687624168726763</v>
+      </c>
+      <c r="K16" s="12">
+        <f>K15*100/K14</f>
+        <v>1.4476229523062767</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="E16" s="12">
-        <f>(E13-B13)/3</f>
+      <c r="C17" s="14"/>
+      <c r="E17" s="12">
+        <f>(E14-B14)/3</f>
         <v>21.240033333333297</v>
       </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="K17" s="12">
+        <f>(K14-H14)/3</f>
+        <v>22.537466666666699</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I28" s="12">
+        <f t="shared" ref="I28" si="4">I13/1000</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>589.79499999999996</v>
-      </c>
-      <c r="C2" s="7">
-        <v>519.84400000000005</v>
-      </c>
-      <c r="D2" s="15">
-        <v>506.86399999999998</v>
-      </c>
-      <c r="E2" s="18">
-        <v>518.553</v>
-      </c>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>508.32</v>
-      </c>
-      <c r="C3" s="7">
-        <v>520.19600000000003</v>
-      </c>
-      <c r="D3" s="16">
-        <v>540.88599999999997</v>
-      </c>
-      <c r="E3" s="18">
-        <v>482.02800000000002</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>457.11399999999998</v>
-      </c>
-      <c r="C4" s="7">
-        <v>510.81299999999999</v>
-      </c>
-      <c r="D4" s="15">
-        <v>519.423</v>
-      </c>
-      <c r="E4" s="19">
-        <v>535.53200000000004</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7">
-        <v>498.12700000000001</v>
-      </c>
-      <c r="C5" s="7">
-        <v>503.85300000000001</v>
-      </c>
-      <c r="D5" s="15">
-        <v>555.923</v>
-      </c>
-      <c r="E5" s="18">
-        <v>529.351</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7">
-        <v>561.79899999999998</v>
-      </c>
-      <c r="C6" s="7">
-        <v>506.60899999999998</v>
-      </c>
-      <c r="D6" s="15">
-        <v>543.85900000000004</v>
-      </c>
-      <c r="E6" s="18">
-        <v>561.32000000000005</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7">
-        <v>430.54500000000002</v>
-      </c>
-      <c r="C7" s="7">
-        <v>501.53</v>
-      </c>
-      <c r="D7" s="15">
-        <v>530.25900000000001</v>
-      </c>
-      <c r="E7" s="18">
-        <v>523.899</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7">
-        <v>440.142</v>
-      </c>
-      <c r="C8" s="7">
-        <v>486.84899999999999</v>
-      </c>
-      <c r="D8" s="15">
-        <v>556.46699999999998</v>
-      </c>
-      <c r="E8" s="18">
-        <v>540.25</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="7">
-        <f>AVERAGE(B2:B8,Sheet1!F101:H101)</f>
-        <v>490.78407171717174</v>
-      </c>
-      <c r="C10" s="7">
-        <f>AVERAGE(C2:C8,'1024B_at_1sec'!C102:E102)</f>
-        <v>507.09914285714291</v>
-      </c>
-      <c r="D10" s="16">
-        <f>AVERAGE(D2:D8,'1024B_at_1sec'!B104:D104)</f>
-        <v>536.24014285714281</v>
-      </c>
-      <c r="E10" s="19">
-        <f>AVERAGE(E2:E8,Sheet1!F104:H104)</f>
-        <v>532.65390000000002</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7">
-        <f>_xlfn.STDEV.P(B2:B8,Sheet1!F101:H101)</f>
-        <v>70.458516442947058</v>
-      </c>
-      <c r="C11" s="7">
-        <f>_xlfn.STDEV.P(C2:C8,Sheet1!B101:D101)</f>
-        <v>40.441137614408753</v>
-      </c>
-      <c r="D11" s="16">
-        <f>_xlfn.STDEV.P(D2:D8,'1024B_at_1sec'!B104:D104)</f>
-        <v>17.145260573186082</v>
-      </c>
-      <c r="E11" s="19">
-        <f>_xlfn.STDEV.P(E2:E8,Sheet1!F104:H104)</f>
-        <v>22.203233347645565</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7">
-        <f t="shared" ref="B12" si="0">B11*100/B10</f>
-        <v>14.356316861797174</v>
-      </c>
-      <c r="C12" s="7">
-        <f>C11*100/C10</f>
-        <v>7.9749962475881366</v>
-      </c>
-      <c r="D12" s="16">
-        <f>D11*100/D10</f>
-        <v>3.197310160674351</v>
-      </c>
-      <c r="E12" s="19">
-        <f>E11*100/E10</f>
-        <v>4.1684165548483856</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13">
-        <f>(E10-B10)/3</f>
-        <v>13.956609427609427</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="7"/>
-    <col min="5" max="5" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>495.93400000000003</v>
-      </c>
-      <c r="C2" s="7">
-        <v>504.21499999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>483.62099999999998</v>
-      </c>
-      <c r="C3" s="7">
-        <v>530.30100000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>501.38900000000001</v>
-      </c>
-      <c r="C4" s="7">
-        <v>489.51600000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7">
-        <v>499.44200000000001</v>
-      </c>
-      <c r="C5" s="7">
-        <v>505.58699999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7">
-        <v>477.87700000000001</v>
-      </c>
-      <c r="C6" s="7">
-        <v>454.37700000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7">
-        <v>508.73599999999999</v>
-      </c>
-      <c r="C7" s="7">
-        <v>493.75900000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7">
-        <v>473.11500000000001</v>
-      </c>
-      <c r="C8" s="7">
-        <v>497.88099999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7">
-        <v>491.59</v>
-      </c>
-      <c r="C9" s="7">
-        <v>515.774</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7">
-        <v>493.42</v>
-      </c>
-      <c r="C10" s="7">
-        <v>523.22299999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7">
-        <v>424.351</v>
-      </c>
-      <c r="C11" s="7">
-        <v>506.71199999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7">
-        <f>AVERAGE(B2:B11)</f>
-        <v>484.94749999999993</v>
-      </c>
-      <c r="C13" s="7">
-        <f>AVERAGE(C2:C11)</f>
-        <v>502.13449999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="7">
-        <f>_xlfn.STDEV.P(B2:B11)</f>
-        <v>22.686143062451144</v>
-      </c>
-      <c r="C14" s="7">
-        <f>_xlfn.STDEV.P(C2:C11)</f>
-        <v>19.973885121578125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="7">
-        <f t="shared" ref="B15" si="0">B14*100/B13</f>
-        <v>4.6780616587261807</v>
-      </c>
-      <c r="C15" s="7">
-        <f>C14*100/C13</f>
-        <v>3.9777958139857206</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="11">
-        <f>(C13-B13)</f>
-        <v>17.187000000000012</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7"/>
-    <col min="7" max="7" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
-        <v>304.40199999999999</v>
-      </c>
-      <c r="C2" s="7">
-        <v>305.10000000000002</v>
-      </c>
-      <c r="D2" s="15">
-        <v>352.89100000000002</v>
-      </c>
-      <c r="E2" s="15">
-        <v>496.38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>296.91000000000003</v>
-      </c>
-      <c r="C3" s="7">
-        <v>292.14499999999998</v>
-      </c>
-      <c r="D3" s="15">
-        <v>293.39999999999998</v>
-      </c>
-      <c r="E3" s="16">
-        <v>294.173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7">
-        <v>311.524</v>
-      </c>
-      <c r="C4" s="7">
-        <v>316.82799999999997</v>
-      </c>
-      <c r="D4" s="15">
-        <v>356.839</v>
-      </c>
-      <c r="E4" s="15">
-        <v>335.15699999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7">
-        <v>282.04500000000002</v>
-      </c>
-      <c r="C5" s="7">
-        <v>299.51299999999998</v>
-      </c>
-      <c r="D5" s="15">
-        <v>320.06099999999998</v>
-      </c>
-      <c r="E5" s="15">
-        <v>338.95299999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7">
-        <v>315.12400000000002</v>
-      </c>
-      <c r="C6" s="7">
-        <v>316.92</v>
-      </c>
-      <c r="D6" s="16">
-        <v>362.31400000000002</v>
-      </c>
-      <c r="E6" s="15">
-        <v>356.96600000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="7">
-        <v>283.71199999999999</v>
-      </c>
-      <c r="C7" s="7">
-        <v>306.84800000000001</v>
-      </c>
-      <c r="D7" s="15">
-        <v>325.887</v>
-      </c>
-      <c r="E7" s="15">
-        <v>277.16000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7">
-        <v>314.13499999999999</v>
-      </c>
-      <c r="C8" s="7">
-        <v>324.21800000000002</v>
-      </c>
-      <c r="D8" s="15">
-        <v>332.31400000000002</v>
-      </c>
-      <c r="E8" s="15">
-        <v>342.43700000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="7">
-        <v>318.67099999999999</v>
-      </c>
-      <c r="C9" s="7">
-        <v>326.17399999999998</v>
-      </c>
-      <c r="D9" s="15">
-        <v>324.04399999999998</v>
-      </c>
-      <c r="E9" s="15">
-        <v>353.15300000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7">
-        <v>290.21199999999999</v>
-      </c>
-      <c r="C10" s="7">
-        <v>322.88200000000001</v>
-      </c>
-      <c r="D10" s="16">
-        <v>338.89400000000001</v>
-      </c>
-      <c r="E10" s="15">
-        <v>345.166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="7">
-        <v>310.02999999999997</v>
-      </c>
-      <c r="C11" s="7">
-        <v>308.44900000000001</v>
-      </c>
-      <c r="D11" s="16">
-        <v>355.67</v>
-      </c>
-      <c r="E11" s="15">
-        <v>328.02499999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="7">
-        <f>AVERAGE(B2:B11)</f>
-        <v>302.67649999999992</v>
-      </c>
-      <c r="C13" s="7">
-        <f>AVERAGE(C2:C11)</f>
-        <v>311.90770000000003</v>
-      </c>
-      <c r="D13" s="16">
-        <f>AVERAGE(D2:D11)</f>
-        <v>336.23139999999995</v>
-      </c>
-      <c r="E13" s="16">
-        <f>AVERAGE(E2:E11)</f>
-        <v>346.75700000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="7">
-        <f>_xlfn.STDEV.P(B2:B11)</f>
-        <v>12.850363467622227</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" ref="C14:E14" si="0">_xlfn.STDEV.P(C2:C11)</f>
-        <v>10.737501637252498</v>
-      </c>
-      <c r="D14" s="16">
-        <f t="shared" si="0"/>
-        <v>20.33313083713378</v>
-      </c>
-      <c r="E14" s="16">
-        <f t="shared" si="0"/>
-        <v>55.415284905881322</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="7">
-        <f t="shared" ref="B15" si="1">B14*100/B13</f>
-        <v>4.2455768675870873</v>
-      </c>
-      <c r="C15" s="7">
-        <f>C14*100/C13</f>
-        <v>3.442525348765836</v>
-      </c>
-      <c r="D15" s="16">
-        <f>D14*100/D13</f>
-        <v>6.0473622740570283</v>
-      </c>
-      <c r="E15" s="16">
-        <f>E14*100/E13</f>
-        <v>15.981014054764959</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11">
-        <f>(E13-B13)/3</f>
-        <v>14.693500000000029</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>